<commit_message>
scrapping inov e aliansi
</commit_message>
<xml_diff>
--- a/thais_imobiliaria/thais_imobiliaria_venda_com_setores.xlsx
+++ b/thais_imobiliaria/thais_imobiliaria_venda_com_setores.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -490,6 +490,1511 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Norte - Águas Claras - DF</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Apartamento</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/apartamento-aguas-claras-2-quartos-78-m/AP16437-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>590000</v>
+      </c>
+      <c r="E2" t="n">
+        <v>7753</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>3</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>OUTRO</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>76.09957435831291</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Norte - Águas Claras - DFWave</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Apartamento</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/apartamento-aguas-claras-2-quartos-98-m/AP16129-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>780000</v>
+      </c>
+      <c r="E3" t="n">
+        <v>98</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>OUTRO</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>7959.183673469388</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Norte - Águas Claras - DFVia Club Residence</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Apartamento</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/apartamento-aguas-claras-3-quartos-96-m/AP15254-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>799000</v>
+      </c>
+      <c r="E4" t="n">
+        <v>9644</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>3</v>
+      </c>
+      <c r="I4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>OUTRO</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>82.8494400663625</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Águas Claras Norte - Águas Claras - DFVitali</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Apartamento</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/apartamento-aguas-claras-2-quartos-64-m/AP15595-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>795000</v>
+      </c>
+      <c r="E5" t="n">
+        <v>64</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>OUTRO</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>12421.875</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Ceilândia Norte - Ceilândia - DFAllegro - Show de Morar</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Apartamento</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/apartamento-ceilandia-3-quartos-88-m/AP17063-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>660000</v>
+      </c>
+      <c r="E6" t="n">
+        <v>877</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>CEILÂNDIA</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>752.5655644241733</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Samambaia Sul - Samambaia - DF</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Área</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/area-samambaia-100-m/AR0009-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>239000</v>
+      </c>
+      <c r="E7" t="n">
+        <v>100</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>SAMAMBAIA</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>2390</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Norte - Águas Claras - DF</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Apartamento</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/apartamento-aguas-claras-4-quartos-164-m/AP17020-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1990000</v>
+      </c>
+      <c r="E8" t="n">
+        <v>164</v>
+      </c>
+      <c r="F8" t="n">
+        <v>4</v>
+      </c>
+      <c r="G8" t="n">
+        <v>4</v>
+      </c>
+      <c r="H8" t="n">
+        <v>3</v>
+      </c>
+      <c r="I8" t="n">
+        <v>3</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>OUTRO</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>12134.14634146341</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Guará II - Guará - DF</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Apartamento</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/apartamento-guara-2-quartos-65-m/AP17084-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>760000</v>
+      </c>
+      <c r="E9" t="n">
+        <v>65</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" t="n">
+        <v>2</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>GUARÁ</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>11692.30769230769</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Guará II - Brasília - DF</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Apartamento</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/apartamento-brasilia-4-quartos-123-m/AP16117-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>1370000</v>
+      </c>
+      <c r="E10" t="n">
+        <v>123</v>
+      </c>
+      <c r="F10" t="n">
+        <v>4</v>
+      </c>
+      <c r="G10" t="n">
+        <v>2</v>
+      </c>
+      <c r="H10" t="n">
+        <v>4</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>GUARÁ</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>11138.21138211382</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Riacho Fundo - Riacho Fundo - DF</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Casa</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/casa-riacho-fundo-4-quartos-150-m/CA6526-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>795000</v>
+      </c>
+      <c r="E11" t="n">
+        <v>150</v>
+      </c>
+      <c r="F11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G11" t="n">
+        <v>3</v>
+      </c>
+      <c r="H11" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" t="n">
+        <v>2</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>OUTRO</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>5300</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Asa Sul - Brasília - DF</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Casa</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/casa-brasilia-4-quartos-431-m/CA6694-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>1990000</v>
+      </c>
+      <c r="E12" t="n">
+        <v>431</v>
+      </c>
+      <c r="F12" t="n">
+        <v>4</v>
+      </c>
+      <c r="G12" t="n">
+        <v>4</v>
+      </c>
+      <c r="H12" t="n">
+        <v>5</v>
+      </c>
+      <c r="I12" t="n">
+        <v>2</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>OUTRO</t>
+        </is>
+      </c>
+      <c r="K12" t="n">
+        <v>4617.169373549884</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Taguatinga Sul - Taguatinga - DF</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Apartamento</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/apartamento-taguatinga-2-quartos-75-m/AP16851-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>260000</v>
+      </c>
+      <c r="E13" t="n">
+        <v>75</v>
+      </c>
+      <c r="F13" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>TAGUATINGA</t>
+        </is>
+      </c>
+      <c r="K13" t="n">
+        <v>3466.666666666667</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Asa Sul - Brasília - DF</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Casa</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/casa-brasilia-4-quartos-100-m/CA6616-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>2500000</v>
+      </c>
+      <c r="E14" t="n">
+        <v>9972</v>
+      </c>
+      <c r="F14" t="n">
+        <v>4</v>
+      </c>
+      <c r="G14" t="n">
+        <v>2</v>
+      </c>
+      <c r="H14" t="n">
+        <v>3</v>
+      </c>
+      <c r="I14" t="n">
+        <v>4</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>OUTRO</t>
+        </is>
+      </c>
+      <c r="K14" t="n">
+        <v>250.7019655034096</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Jardins Mangueiral - São Sebastião - DF</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Casa</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/casa-sao-sebastiao-3-quartos-236-m/CA6584-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>499000</v>
+      </c>
+      <c r="E15" t="n">
+        <v>236</v>
+      </c>
+      <c r="F15" t="n">
+        <v>3</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" t="n">
+        <v>3</v>
+      </c>
+      <c r="I15" t="n">
+        <v>2</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>OUTRO</t>
+        </is>
+      </c>
+      <c r="K15" t="n">
+        <v>2114.406779661017</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Ceilândia Sul - Ceilândia - DF</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Prédio</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/predio-ceilandia-420-m/PR0260-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>1150000</v>
+      </c>
+      <c r="E16" t="n">
+        <v>420</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>6</v>
+      </c>
+      <c r="I16" t="n">
+        <v>2</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>CEILÂNDIA</t>
+        </is>
+      </c>
+      <c r="K16" t="n">
+        <v>2738.095238095238</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Guará I - Guará - DF</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Casa</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/casa-guara-4-quartos-160-m/CA6417-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>749000</v>
+      </c>
+      <c r="E17" t="n">
+        <v>160</v>
+      </c>
+      <c r="F17" t="n">
+        <v>4</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" t="n">
+        <v>3</v>
+      </c>
+      <c r="I17" t="n">
+        <v>3</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>GUARÁ</t>
+        </is>
+      </c>
+      <c r="K17" t="n">
+        <v>4681.25</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Sudoeste - Brasília - DF</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Loja</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/loja-brasilia-28-m/LO1083-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>450000</v>
+      </c>
+      <c r="E18" t="n">
+        <v>28</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
+        <v>1</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>OUTRO</t>
+        </is>
+      </c>
+      <c r="K18" t="n">
+        <v>16071.42857142857</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Guará II - Guará - DF</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Casa</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/casa-guara-3-quartos-128-m/CA6535-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>850000</v>
+      </c>
+      <c r="E19" t="n">
+        <v>128</v>
+      </c>
+      <c r="F19" t="n">
+        <v>3</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" t="n">
+        <v>2</v>
+      </c>
+      <c r="I19" t="n">
+        <v>3</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>GUARÁ</t>
+        </is>
+      </c>
+      <c r="K19" t="n">
+        <v>6640.625</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Quadras Econômicas Lúcio Costa - Guará - DF</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Apartamento</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/apartamento-guara-2-quartos-59-m/AP16726-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>370000</v>
+      </c>
+      <c r="E20" t="n">
+        <v>59</v>
+      </c>
+      <c r="F20" t="n">
+        <v>2</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>GUARÁ</t>
+        </is>
+      </c>
+      <c r="K20" t="n">
+        <v>6271.186440677966</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Noroeste - Brasília - DF</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Apartamento</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/apartamento-brasilia-2-quartos-82-m/AP16946-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>1300000</v>
+      </c>
+      <c r="E21" t="n">
+        <v>82</v>
+      </c>
+      <c r="F21" t="n">
+        <v>2</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1</v>
+      </c>
+      <c r="H21" t="n">
+        <v>3</v>
+      </c>
+      <c r="I21" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>OUTRO</t>
+        </is>
+      </c>
+      <c r="K21" t="n">
+        <v>15853.65853658537</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Guará II - Guará - DF</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Casa</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/casa-guara-4-quartos-400-m/CA6670-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>1850000</v>
+      </c>
+      <c r="E22" t="n">
+        <v>400</v>
+      </c>
+      <c r="F22" t="n">
+        <v>4</v>
+      </c>
+      <c r="G22" t="n">
+        <v>4</v>
+      </c>
+      <c r="H22" t="n">
+        <v>5</v>
+      </c>
+      <c r="I22" t="n">
+        <v>3</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>GUARÁ</t>
+        </is>
+      </c>
+      <c r="K22" t="n">
+        <v>4625</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Setor Habitacional Jardim Botânico - Brasília - DF</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Casa</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/casa-brasilia-3-quartos-360-m/CA6674-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>1200000</v>
+      </c>
+      <c r="E23" t="n">
+        <v>360</v>
+      </c>
+      <c r="F23" t="n">
+        <v>3</v>
+      </c>
+      <c r="G23" t="n">
+        <v>2</v>
+      </c>
+      <c r="H23" t="n">
+        <v>4</v>
+      </c>
+      <c r="I23" t="n">
+        <v>4</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>OUTRO</t>
+        </is>
+      </c>
+      <c r="K23" t="n">
+        <v>3333.333333333333</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Park Way - Brasília - DF</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Casa</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/casa-brasilia-7-quartos-550-m/CA6675-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>3600000</v>
+      </c>
+      <c r="E24" t="n">
+        <v>550</v>
+      </c>
+      <c r="F24" t="n">
+        <v>7</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1</v>
+      </c>
+      <c r="H24" t="n">
+        <v>7</v>
+      </c>
+      <c r="I24" t="n">
+        <v>7</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>OUTRO</t>
+        </is>
+      </c>
+      <c r="K24" t="n">
+        <v>6545.454545454545</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Guará I - Guará - DF</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Apartamento</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/apartamento-guara-2-quartos-39-m/AP16774-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>159000</v>
+      </c>
+      <c r="E25" t="n">
+        <v>39</v>
+      </c>
+      <c r="F25" t="n">
+        <v>2</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>GUARÁ</t>
+        </is>
+      </c>
+      <c r="K25" t="n">
+        <v>4076.923076923077</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Asa Sul - Brasília - DF</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Apartamento</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/apartamento-brasilia-2-quartos-55-m/AP17025-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>560000</v>
+      </c>
+      <c r="E26" t="n">
+        <v>55</v>
+      </c>
+      <c r="F26" t="n">
+        <v>2</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>OUTRO</t>
+        </is>
+      </c>
+      <c r="K26" t="n">
+        <v>10181.81818181818</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Guará I - Guará - DF</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Casa</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/casa-guara-2-quartos-120-m/CA6377-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>580000</v>
+      </c>
+      <c r="E27" t="n">
+        <v>120</v>
+      </c>
+      <c r="F27" t="n">
+        <v>2</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>1</v>
+      </c>
+      <c r="I27" t="n">
+        <v>3</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>GUARÁ</t>
+        </is>
+      </c>
+      <c r="K27" t="n">
+        <v>4833.333333333333</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Park Sul - Brasília - DFVenice Park Residence Service</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Apartamento</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/apartamento-brasilia-1-quarto-26-m/AP16425-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>400000</v>
+      </c>
+      <c r="E28" t="n">
+        <v>26</v>
+      </c>
+      <c r="F28" t="n">
+        <v>1</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1</v>
+      </c>
+      <c r="H28" t="n">
+        <v>1</v>
+      </c>
+      <c r="I28" t="n">
+        <v>1</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>OUTRO</t>
+        </is>
+      </c>
+      <c r="K28" t="n">
+        <v>15384.61538461538</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Park Sul - Brasília - DFVenice Park Residence Service</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Apartamento</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/apartamento-brasilia-1-quarto-26-m/AP16426-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>399500</v>
+      </c>
+      <c r="E29" t="n">
+        <v>262</v>
+      </c>
+      <c r="F29" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>1</v>
+      </c>
+      <c r="I29" t="n">
+        <v>1</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>OUTRO</t>
+        </is>
+      </c>
+      <c r="K29" t="n">
+        <v>1524.809160305344</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Águas Claras Norte - Águas Claras - DFEasy</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Apartamento</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/apartamento-aguas-claras-2-quartos-54-m/AP16646-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>539990</v>
+      </c>
+      <c r="E30" t="n">
+        <v>54</v>
+      </c>
+      <c r="F30" t="n">
+        <v>2</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1</v>
+      </c>
+      <c r="H30" t="n">
+        <v>2</v>
+      </c>
+      <c r="I30" t="n">
+        <v>1</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>OUTRO</t>
+        </is>
+      </c>
+      <c r="K30" t="n">
+        <v>9999.814814814816</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Asa Norte - Brasília - DF</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Apartamento</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/apartamento-brasilia-3-quartos-95-m/AP16546-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>780000</v>
+      </c>
+      <c r="E31" t="n">
+        <v>95</v>
+      </c>
+      <c r="F31" t="n">
+        <v>3</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>1</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>OUTRO</t>
+        </is>
+      </c>
+      <c r="K31" t="n">
+        <v>8210.526315789473</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Núcleo Bandeirante - Núcleo Bandeirante - DF</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Apartamento</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/apartamento-nucleo-bandeirante-1-quarto-29-m/AP16461-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>149000</v>
+      </c>
+      <c r="E32" t="n">
+        <v>2932</v>
+      </c>
+      <c r="F32" t="n">
+        <v>1</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>OUTRO</t>
+        </is>
+      </c>
+      <c r="K32" t="n">
+        <v>50.81855388813097</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Guará II - Brasília - DF</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Casa</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/casa-brasilia-4-quartos-300-m/CA6473-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>1490000</v>
+      </c>
+      <c r="E33" t="n">
+        <v>300</v>
+      </c>
+      <c r="F33" t="n">
+        <v>4</v>
+      </c>
+      <c r="G33" t="n">
+        <v>2</v>
+      </c>
+      <c r="H33" t="n">
+        <v>4</v>
+      </c>
+      <c r="I33" t="n">
+        <v>3</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>GUARÁ</t>
+        </is>
+      </c>
+      <c r="K33" t="n">
+        <v>4966.666666666667</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Sudoeste - Brasília - DF</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Apartamento</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/apartamento-brasilia-1-quarto-24-m/AP17010-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>384000</v>
+      </c>
+      <c r="E34" t="n">
+        <v>24</v>
+      </c>
+      <c r="F34" t="n">
+        <v>1</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="n">
+        <v>1</v>
+      </c>
+      <c r="I34" t="n">
+        <v>1</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>OUTRO</t>
+        </is>
+      </c>
+      <c r="K34" t="n">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Taguatinga Norte - Taguatinga - DF</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Casa</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/casa-taguatinga-5-quartos-120-m/CA6419-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>429000</v>
+      </c>
+      <c r="E35" t="n">
+        <v>120</v>
+      </c>
+      <c r="F35" t="n">
+        <v>5</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1</v>
+      </c>
+      <c r="H35" t="n">
+        <v>2</v>
+      </c>
+      <c r="I35" t="n">
+        <v>1</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>TAGUATINGA</t>
+        </is>
+      </c>
+      <c r="K35" t="n">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Guará I - Guará - DF</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Apartamento</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>https://www.thaisimobiliaria.com.br/imovel/apartamento-guara-2-quartos-41-m/AP16700-TH?from=sale</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>344900</v>
+      </c>
+      <c r="E36" t="n">
+        <v>4126</v>
+      </c>
+      <c r="F36" t="n">
+        <v>2</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" t="n">
+        <v>1</v>
+      </c>
+      <c r="I36" t="n">
+        <v>1</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>GUARÁ</t>
+        </is>
+      </c>
+      <c r="K36" t="n">
+        <v>83.59185651963161</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>